<commit_message>
seed database updated for group and type
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/09-BulkUploadMachineGroup.xlsx
+++ b/documents/templates/bulk-upload/09-BulkUploadMachineGroup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEC8463A-16EA-1E4C-8DBA-CEADAC6D05FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD1BBAE-B124-3444-923E-52FC0CAFBDC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{03CB352A-59C4-E548-9F5B-8794D5B56636}"/>
   </bookViews>
@@ -31,9 +31,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Machine Group</t>
+  </si>
+  <si>
+    <t>ASSY</t>
+  </si>
+  <si>
+    <t>BOMAR</t>
+  </si>
+  <si>
+    <t>BOMAR4</t>
+  </si>
+  <si>
+    <t>BOOMAR</t>
+  </si>
+  <si>
+    <t>E50</t>
+  </si>
+  <si>
+    <t>ITC</t>
+  </si>
+  <si>
+    <t>PCM_GROUP_1</t>
+  </si>
+  <si>
+    <t>PLASMA</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>SCM_GROUP_1</t>
+  </si>
+  <si>
+    <t>SHEARING</t>
+  </si>
+  <si>
+    <t>SLOT COMMONISATION</t>
+  </si>
+  <si>
+    <t>SMC_GROUP_1</t>
+  </si>
+  <si>
+    <t>SMS_GROUP_1</t>
+  </si>
+  <si>
+    <t>SOCO</t>
+  </si>
+  <si>
+    <t>TBV_GROUP_1</t>
+  </si>
+  <si>
+    <t>TCA_GROUP_1</t>
+  </si>
+  <si>
+    <t>TCM_GROUP_1</t>
+  </si>
+  <si>
+    <t>TRUMPF</t>
+  </si>
+  <si>
+    <t>Machine Type</t>
+  </si>
+  <si>
+    <t>Band saw</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -385,17 +454,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6603046D-2B86-B141-B65D-D932A8F5B98E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>